<commit_message>
commit. added new code for pwm-ing an rgb led
</commit_message>
<xml_diff>
--- a/AtTinyTests.xlsx
+++ b/AtTinyTests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="19980" windowHeight="8835"/>
+    <workbookView xWindow="675" yWindow="255" windowWidth="19980" windowHeight="8835"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,12 +16,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Atlas Sci</t>
   </si>
   <si>
     <t>AtTiny</t>
+  </si>
+  <si>
+    <t>TDSez</t>
+  </si>
+  <si>
+    <t>cal1 (220)</t>
+  </si>
+  <si>
+    <t>cal2 (3000)</t>
   </si>
 </sst>
 </file>
@@ -361,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -372,15 +381,186 @@
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>41479</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>60</v>
+      </c>
+      <c r="C2">
+        <v>145</v>
+      </c>
+      <c r="D2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>110</v>
+      </c>
+      <c r="C3">
+        <v>259</v>
+      </c>
+      <c r="D3">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>150</v>
+      </c>
+      <c r="C4">
+        <v>547</v>
+      </c>
+      <c r="D4">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>183</v>
+      </c>
+      <c r="C5">
+        <v>797</v>
+      </c>
+      <c r="D5">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>325</v>
+      </c>
+      <c r="C6">
+        <v>1250</v>
+      </c>
+      <c r="D6">
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>429</v>
+      </c>
+      <c r="C7">
+        <v>1531</v>
+      </c>
+      <c r="D7">
+        <v>1778</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>521</v>
+      </c>
+      <c r="C8">
+        <v>1695</v>
+      </c>
+      <c r="D8">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>739</v>
+      </c>
+      <c r="C9">
+        <v>2039</v>
+      </c>
+      <c r="D9">
+        <v>2471</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1070</v>
+      </c>
+      <c r="C10">
+        <v>2970</v>
+      </c>
+      <c r="D10">
+        <v>2906</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>863</v>
+      </c>
+      <c r="C11">
+        <v>2722</v>
+      </c>
+      <c r="D11">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>114</v>
+      </c>
+      <c r="C12">
+        <v>220</v>
+      </c>
+      <c r="D12">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>1110</v>
+      </c>
+      <c r="C13">
+        <v>3000</v>
+      </c>
+      <c r="D13">
+        <v>3100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>